<commit_message>
Aggiornamento dei commenti e del codice 02.08.2017
Il commit precedente e' errato ho fatto l'upload dei file vecchi.
</commit_message>
<xml_diff>
--- a/Esercizio1/Esercizio1.xlsx
+++ b/Esercizio1/Esercizio1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita\Method and Tools\ProgettoSacile\Esercizio1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Università\Magistrale\Methods And Tools For Industrial Automation\Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,7 +691,7 @@
   <dimension ref="B1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>